<commit_message>
Log-transformed Count NMDS for all sites
</commit_message>
<xml_diff>
--- a/Part b (09-19)/NMDS (Count) - all sites - spatial question/count_combined_allsites.xlsx
+++ b/Part b (09-19)/NMDS (Count) - all sites - spatial question/count_combined_allsites.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub Projects\thesis_codes\Part b (09-19)\NMDS (Count) - all sites - spatial question\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55467396-FD70-406A-9CD9-50818E2F01A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601BF269-78F7-41A4-9E82-426318B544E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30720" yWindow="1920" windowWidth="16200" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHIRAE G" sheetId="4" r:id="rId1"/>
     <sheet name="CHIRAE F" sheetId="6" r:id="rId2"/>
     <sheet name="PC ORD CHIRAE F" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CHIRAE G'!$A$1:$C$47</definedName>
+  </definedNames>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1413,8 +1416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E1BEC9-E474-4887-9D77-6C2ED8884D8B}">
   <dimension ref="A1:IG47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35499,6 +35502,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C47" xr:uid="{F4E1BEC9-E474-4887-9D77-6C2ED8884D8B}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D1:HS1">
     <cfRule type="duplicateValues" dxfId="5" priority="2"/>
@@ -61295,9 +61299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9F43FB-E229-4B7A-802A-753A16EAAB2C}">
   <dimension ref="A1:DP47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>